<commit_message>
a whole bunch of changes that has not been pushed
</commit_message>
<xml_diff>
--- a/Documentation/Risk Assesment.xlsx
+++ b/Documentation/Risk Assesment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/College - Uni/Uni Project/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{E30EBA15-0AE7-40FB-99FC-BDA8F347B9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF0F05A2-D191-44B2-B6E5-D99E5A2AD4C1}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{E30EBA15-0AE7-40FB-99FC-BDA8F347B9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D2CEC57-0BFD-4F23-B9AE-B39DDCE63954}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2018D5C7-2B3B-45DA-AB2A-2CEC4335F664}"/>
   </bookViews>
@@ -117,9 +117,6 @@
     <t>Safety</t>
   </si>
   <si>
-    <t>Food health and safety requirements</t>
-  </si>
-  <si>
     <t>Development</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Optimistic Schedule</t>
+  </si>
+  <si>
+    <t>Health and Safety requirements</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -716,7 +716,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>7</v>
@@ -725,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>6</v>
@@ -756,7 +756,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>12</v>
@@ -765,7 +765,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>12</v>
@@ -785,7 +785,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>7</v>
@@ -805,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>13</v>
@@ -825,7 +825,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -896,16 +896,16 @@
         <v>29</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>2</v>
@@ -931,10 +931,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>7</v>
@@ -943,7 +943,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>3</v>
@@ -966,10 +966,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>12</v>
@@ -978,7 +978,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -986,10 +986,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>12</v>
@@ -998,7 +998,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>